<commit_message>
CleanCode sobre 1er Semana
</commit_message>
<xml_diff>
--- a/Semana-1/files/Taxes-Gestion.xlsx
+++ b/Semana-1/files/Taxes-Gestion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Automation Anywhere Files\Automation Anywhere\My Tasks\Semana-1\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13932A92-A6EF-4E28-9A16-95BAAEEDEB82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EC61FC-E5FB-4FB1-BB45-C4558ECDFAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,7 +623,7 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-8785-4E95-9F27-3DF2E753B134}"/>
+                <c16:uniqueId val="{00000001-374A-4253-9D24-10FB891F2C35}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -640,7 +640,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-8785-4E95-9F27-3DF2E753B134}"/>
+                <c16:uniqueId val="{00000003-374A-4253-9D24-10FB891F2C35}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -657,7 +657,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-8785-4E95-9F27-3DF2E753B134}"/>
+                <c16:uniqueId val="{00000005-374A-4253-9D24-10FB891F2C35}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -674,7 +674,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-8785-4E95-9F27-3DF2E753B134}"/>
+                <c16:uniqueId val="{00000007-374A-4253-9D24-10FB891F2C35}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -691,7 +691,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-8785-4E95-9F27-3DF2E753B134}"/>
+                <c16:uniqueId val="{00000009-374A-4253-9D24-10FB891F2C35}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -708,7 +708,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-8785-4E95-9F27-3DF2E753B134}"/>
+                <c16:uniqueId val="{0000000B-374A-4253-9D24-10FB891F2C35}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -817,7 +817,7 @@
               </c15:filteredCategoryTitle>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-8785-4E95-9F27-3DF2E753B134}"/>
+              <c16:uniqueId val="{0000000C-374A-4253-9D24-10FB891F2C35}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1057,7 +1057,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4C90-4D79-9861-F09D0D7A3DE5}"/>
+              <c16:uniqueId val="{00000000-9F78-4188-AFC6-D9BBE04297DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1071,12 +1071,12 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="26921279"/>
-        <c:axId val="61833804"/>
+        <c:axId val="98513911"/>
+        <c:axId val="29017467"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="26921279"/>
+        <c:axId val="98513911"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1105,7 +1105,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61833804"/>
+        <c:crossAx val="29017467"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1113,7 +1113,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61833804"/>
+        <c:axId val="29017467"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1151,7 +1151,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26921279"/>
+        <c:crossAx val="98513911"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1372,7 +1372,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7C2F-4FD0-A0CA-5382DD39CB1C}"/>
+              <c16:uniqueId val="{00000000-5617-4564-97A3-F0D5BCB31468}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1386,12 +1386,12 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="91496197"/>
-        <c:axId val="62044829"/>
+        <c:axId val="16212397"/>
+        <c:axId val="79036902"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="91496197"/>
+        <c:axId val="16212397"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,7 +1420,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62044829"/>
+        <c:crossAx val="79036902"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1428,7 +1428,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62044829"/>
+        <c:axId val="79036902"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1466,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91496197"/>
+        <c:crossAx val="16212397"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1687,7 +1687,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2152-4455-8ED4-3E8388F3B790}"/>
+              <c16:uniqueId val="{00000000-4412-4B15-86E0-4312DB8A9156}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1701,12 +1701,12 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="18592814"/>
-        <c:axId val="55271465"/>
+        <c:axId val="44751643"/>
+        <c:axId val="4944694"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="18592814"/>
+        <c:axId val="44751643"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,7 +1735,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55271465"/>
+        <c:crossAx val="4944694"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1743,7 +1743,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55271465"/>
+        <c:axId val="4944694"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1781,7 +1781,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18592814"/>
+        <c:crossAx val="44751643"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1975,7 +1975,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6F4F-41C1-ADFC-097995B041C2}"/>
+              <c16:uniqueId val="{00000000-5918-4F54-A8ED-B0864300B237}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1989,12 +1989,12 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="60112183"/>
-        <c:axId val="22150843"/>
+        <c:axId val="86488636"/>
+        <c:axId val="91040738"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="60112183"/>
+        <c:axId val="86488636"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2023,7 +2023,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22150843"/>
+        <c:crossAx val="91040738"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2031,7 +2031,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22150843"/>
+        <c:axId val="91040738"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,7 +2069,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60112183"/>
+        <c:crossAx val="86488636"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2166,7 +2166,7 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-2E7C-462D-A6ED-78FBEDC2D1FA}"/>
+                <c16:uniqueId val="{00000001-DE20-46D2-858A-0D5A52D1EA20}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2183,7 +2183,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-2E7C-462D-A6ED-78FBEDC2D1FA}"/>
+                <c16:uniqueId val="{00000003-DE20-46D2-858A-0D5A52D1EA20}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2200,7 +2200,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-2E7C-462D-A6ED-78FBEDC2D1FA}"/>
+                <c16:uniqueId val="{00000005-DE20-46D2-858A-0D5A52D1EA20}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2217,7 +2217,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-2E7C-462D-A6ED-78FBEDC2D1FA}"/>
+                <c16:uniqueId val="{00000007-DE20-46D2-858A-0D5A52D1EA20}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2234,7 +2234,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-2E7C-462D-A6ED-78FBEDC2D1FA}"/>
+                <c16:uniqueId val="{00000009-DE20-46D2-858A-0D5A52D1EA20}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2251,7 +2251,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-2E7C-462D-A6ED-78FBEDC2D1FA}"/>
+                <c16:uniqueId val="{0000000B-DE20-46D2-858A-0D5A52D1EA20}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2360,7 +2360,7 @@
               </c15:filteredCategoryTitle>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-2E7C-462D-A6ED-78FBEDC2D1FA}"/>
+              <c16:uniqueId val="{0000000C-DE20-46D2-858A-0D5A52D1EA20}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2476,7 +2476,7 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-9927-4377-8F0B-7B55EB608948}"/>
+                <c16:uniqueId val="{00000001-D957-4881-9A88-C5288B714126}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2493,7 +2493,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-9927-4377-8F0B-7B55EB608948}"/>
+                <c16:uniqueId val="{00000003-D957-4881-9A88-C5288B714126}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2510,7 +2510,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-9927-4377-8F0B-7B55EB608948}"/>
+                <c16:uniqueId val="{00000005-D957-4881-9A88-C5288B714126}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2527,7 +2527,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-9927-4377-8F0B-7B55EB608948}"/>
+                <c16:uniqueId val="{00000007-D957-4881-9A88-C5288B714126}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2544,7 +2544,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-9927-4377-8F0B-7B55EB608948}"/>
+                <c16:uniqueId val="{00000009-D957-4881-9A88-C5288B714126}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2561,7 +2561,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-9927-4377-8F0B-7B55EB608948}"/>
+                <c16:uniqueId val="{0000000B-D957-4881-9A88-C5288B714126}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2670,7 +2670,7 @@
               </c15:filteredCategoryTitle>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-9927-4377-8F0B-7B55EB608948}"/>
+              <c16:uniqueId val="{0000000C-D957-4881-9A88-C5288B714126}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2786,7 +2786,7 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-EE66-4B4F-A5EE-E7AF61E1817C}"/>
+                <c16:uniqueId val="{00000001-8CAA-4A78-AFFC-118B7AAC0232}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2803,7 +2803,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-EE66-4B4F-A5EE-E7AF61E1817C}"/>
+                <c16:uniqueId val="{00000003-8CAA-4A78-AFFC-118B7AAC0232}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2820,7 +2820,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-EE66-4B4F-A5EE-E7AF61E1817C}"/>
+                <c16:uniqueId val="{00000005-8CAA-4A78-AFFC-118B7AAC0232}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2837,7 +2837,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-EE66-4B4F-A5EE-E7AF61E1817C}"/>
+                <c16:uniqueId val="{00000007-8CAA-4A78-AFFC-118B7AAC0232}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2854,7 +2854,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-EE66-4B4F-A5EE-E7AF61E1817C}"/>
+                <c16:uniqueId val="{00000009-8CAA-4A78-AFFC-118B7AAC0232}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2871,7 +2871,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-EE66-4B4F-A5EE-E7AF61E1817C}"/>
+                <c16:uniqueId val="{0000000B-8CAA-4A78-AFFC-118B7AAC0232}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2980,7 +2980,7 @@
               </c15:filteredCategoryTitle>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-EE66-4B4F-A5EE-E7AF61E1817C}"/>
+              <c16:uniqueId val="{0000000C-8CAA-4A78-AFFC-118B7AAC0232}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3096,7 +3096,7 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-1549-4C00-BAC7-B2F04CF0988C}"/>
+                <c16:uniqueId val="{00000001-EDC7-4445-956E-ED0500537E34}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3113,7 +3113,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-1549-4C00-BAC7-B2F04CF0988C}"/>
+                <c16:uniqueId val="{00000003-EDC7-4445-956E-ED0500537E34}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3130,7 +3130,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-1549-4C00-BAC7-B2F04CF0988C}"/>
+                <c16:uniqueId val="{00000005-EDC7-4445-956E-ED0500537E34}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3147,7 +3147,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-1549-4C00-BAC7-B2F04CF0988C}"/>
+                <c16:uniqueId val="{00000007-EDC7-4445-956E-ED0500537E34}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3164,7 +3164,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-1549-4C00-BAC7-B2F04CF0988C}"/>
+                <c16:uniqueId val="{00000009-EDC7-4445-956E-ED0500537E34}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3181,7 +3181,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-1549-4C00-BAC7-B2F04CF0988C}"/>
+                <c16:uniqueId val="{0000000B-EDC7-4445-956E-ED0500537E34}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3290,7 +3290,7 @@
               </c15:filteredCategoryTitle>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-1549-4C00-BAC7-B2F04CF0988C}"/>
+              <c16:uniqueId val="{0000000C-EDC7-4445-956E-ED0500537E34}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3417,7 +3417,7 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-47BF-473D-8AA0-D29EF97E1E46}"/>
+                <c16:uniqueId val="{00000001-65D2-4AC4-A720-AD59D47410AF}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3434,7 +3434,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-47BF-473D-8AA0-D29EF97E1E46}"/>
+                <c16:uniqueId val="{00000003-65D2-4AC4-A720-AD59D47410AF}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3451,7 +3451,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-47BF-473D-8AA0-D29EF97E1E46}"/>
+                <c16:uniqueId val="{00000005-65D2-4AC4-A720-AD59D47410AF}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3468,7 +3468,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-47BF-473D-8AA0-D29EF97E1E46}"/>
+                <c16:uniqueId val="{00000007-65D2-4AC4-A720-AD59D47410AF}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3485,7 +3485,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-47BF-473D-8AA0-D29EF97E1E46}"/>
+                <c16:uniqueId val="{00000009-65D2-4AC4-A720-AD59D47410AF}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3502,7 +3502,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-47BF-473D-8AA0-D29EF97E1E46}"/>
+                <c16:uniqueId val="{0000000B-65D2-4AC4-A720-AD59D47410AF}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -3580,7 +3580,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-47BF-473D-8AA0-D29EF97E1E46}"/>
+              <c16:uniqueId val="{0000000C-65D2-4AC4-A720-AD59D47410AF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3820,7 +3820,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F6C6-4D36-8C5C-4D9624C1A2DF}"/>
+              <c16:uniqueId val="{00000000-5AA1-4C86-BDEF-71BFAE95D03E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3834,12 +3834,12 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="26708225"/>
-        <c:axId val="22792773"/>
+        <c:axId val="65839209"/>
+        <c:axId val="67364118"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="26708225"/>
+        <c:axId val="65839209"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3868,7 +3868,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22792773"/>
+        <c:crossAx val="67364118"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3876,7 +3876,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22792773"/>
+        <c:axId val="67364118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3914,7 +3914,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26708225"/>
+        <c:crossAx val="65839209"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4135,7 +4135,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E762-4872-9DEE-7A66E22751B8}"/>
+              <c16:uniqueId val="{00000002-464A-4469-B8EE-EE54DA2766C7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4149,12 +4149,12 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="37534248"/>
-        <c:axId val="60603187"/>
+        <c:axId val="28864574"/>
+        <c:axId val="45429655"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="37534248"/>
+        <c:axId val="28864574"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4183,7 +4183,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60603187"/>
+        <c:crossAx val="45429655"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4191,7 +4191,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60603187"/>
+        <c:axId val="45429655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4229,7 +4229,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37534248"/>
+        <c:crossAx val="28864574"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4450,7 +4450,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-61C7-476E-9891-73A774125D37}"/>
+              <c16:uniqueId val="{00000000-28D2-42DB-9045-2480E6AD416B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4464,12 +4464,12 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="92226294"/>
-        <c:axId val="92480440"/>
+        <c:axId val="98623388"/>
+        <c:axId val="7360909"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="92226294"/>
+        <c:axId val="98623388"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4498,7 +4498,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92480440"/>
+        <c:crossAx val="7360909"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4506,7 +4506,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92480440"/>
+        <c:axId val="7360909"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4544,7 +4544,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92226294"/>
+        <c:crossAx val="98623388"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6221,7 +6221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:S52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>

</xml_diff>